<commit_message>
Spell check and standardization
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['Seat #1 is occupied by Basma', 'Seat #2 is occupied by Kelli', 'Seat #3 is occupied by Muntadher', 'Seat #4 is occupied by Veena', 'Seat #5 is occupied by Zelimkhan']</t>
+          <t>['Seat #1 is occupied by Izabela', 'Seat #2 is occupied by Maarten', 'Seat #3 is occupied by Petra', 'Seat #4 is occupied by Zelimkhan']</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Seat #1 is occupied by Anastasiia', 'Seat #2 is occupied by Minh Duc', 'Seat #3 is occupied by Nicolaas', 'Seat #4 is occupied by Wouter', 'Seat #5 is unoccupied']</t>
+          <t>['Seat #1 is occupied by Adheeba', 'Seat #2 is occupied by Kevin', 'Seat #3 is occupied by Soha', 'Seat #4 is occupied by Wouter']</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['Seat #1 is occupied by Adheeba', 'Seat #2 is occupied by Majid', 'Seat #3 is occupied by Rasmita', 'Seat #4 is occupied by Urson', 'Seat #5 is occupied by Yusra']</t>
+          <t>['Seat #1 is occupied by Kelli', 'Seat #2 is occupied by Minh Duc', 'Seat #3 is occupied by Nicolaas', 'Seat #4 is unoccupied']</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['Seat #1 is occupied by Izabela', 'Seat #2 is occupied by Maarten', 'Seat #3 is occupied by Petra', 'Seat #4 is occupied by Soha', 'Seat #5 is unoccupied']</t>
+          <t>['Seat #1 is occupied by Anastasiia', 'Seat #2 is occupied by Muntadher', 'Seat #3 is occupied by Rasmita', 'Seat #4 is occupied by Yusra']</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Seat #1 is occupied by Ihor', 'Seat #2 is occupied by Levin', 'Seat #3 is occupied by Moustafa', 'Seat #4 is occupied by Yeliz', 'Seat #5 is unoccupied']</t>
+          <t>['Seat #1 is occupied by Ihor', 'Seat #2 is occupied by Levin', 'Seat #3 is occupied by Tom', 'Seat #4 is occupied by Veena']</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Seat #1 is occupied by Dhrisya', 'Seat #2 is occupied by Kevin', 'Seat #3 is occupied by Rik', 'Seat #4 is occupied by Tom', 'Seat #5 is unoccupied']</t>
+          <t>['Seat #1 is occupied by Dhrisya', 'Seat #2 is occupied by Majid', 'Seat #3 is occupied by Rik', 'Seat #4 is occupied by Yeliz']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Table 7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['Seat #1 is occupied by Basma', 'Seat #2 is occupied by Moustafa', 'Seat #3 is occupied by Urson', 'Seat #4 is unoccupied']</t>
         </is>
       </c>
     </row>

</xml_diff>